<commit_message>
add new file of plane's color
</commit_message>
<xml_diff>
--- a/仓库/Group_data_Hao_Fu_03.xlsx
+++ b/仓库/Group_data_Hao_Fu_03.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Bristol\computer program\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jelly Jinzhe Liu\Desktop\Big-Project\仓库\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5FF09556-8B20-4CF0-9A56-09F27544F04B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CD64741-64A1-45BC-916F-7B5E14B289DE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{7CE85991-CB1E-4B55-99E7-6D0342950372}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{7CE85991-CB1E-4B55-99E7-6D0342950372}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,6 +20,15 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
@@ -144,18 +153,18 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -506,13 +515,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48412224-5426-4BC5-8378-DF44F3ECC56A}">
   <dimension ref="A1:Z39"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:D5"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C39" sqref="C39:Z39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:26">
       <c r="A1" s="1" t="s">
         <v>31</v>
       </c>
@@ -525,7 +534,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:26">
       <c r="A2" s="1" t="s">
         <v>32</v>
       </c>
@@ -535,7 +544,7 @@
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:26">
       <c r="H3" s="1" t="s">
         <v>34</v>
       </c>
@@ -546,7 +555,7 @@
       <c r="M3" s="1"/>
       <c r="N3" s="1"/>
     </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:26">
       <c r="A5" s="1" t="s">
         <v>35</v>
       </c>
@@ -554,7 +563,7 @@
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
     </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:26">
       <c r="C7">
         <v>1.1000000000000001</v>
       </c>
@@ -628,7 +637,7 @@
         <v>8.3000000000000007</v>
       </c>
     </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:26">
       <c r="B8" t="s">
         <v>0</v>
       </c>
@@ -705,7 +714,7 @@
         <v>991</v>
       </c>
     </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:26">
       <c r="B9" t="s">
         <v>1</v>
       </c>
@@ -782,7 +791,7 @@
         <v>593</v>
       </c>
     </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:26">
       <c r="B10" t="s">
         <v>2</v>
       </c>
@@ -859,7 +868,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:26">
       <c r="B11" t="s">
         <v>3</v>
       </c>
@@ -936,7 +945,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:26">
       <c r="B12" t="s">
         <v>4</v>
       </c>
@@ -1013,7 +1022,7 @@
         <v>1590</v>
       </c>
     </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:26">
       <c r="B13" t="s">
         <v>5</v>
       </c>
@@ -1090,7 +1099,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:26">
       <c r="B14" t="s">
         <v>6</v>
       </c>
@@ -1167,7 +1176,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:26">
       <c r="B15" t="s">
         <v>7</v>
       </c>
@@ -1244,7 +1253,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="16" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:26">
       <c r="B16" t="s">
         <v>8</v>
       </c>
@@ -1321,7 +1330,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="17" spans="2:26" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:26">
       <c r="B17" t="s">
         <v>9</v>
       </c>
@@ -1398,7 +1407,7 @@
         <v>1276</v>
       </c>
     </row>
-    <row r="18" spans="2:26" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:26">
       <c r="B18" t="s">
         <v>10</v>
       </c>
@@ -1475,7 +1484,7 @@
         <v>944</v>
       </c>
     </row>
-    <row r="19" spans="2:26" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:26">
       <c r="B19" t="s">
         <v>11</v>
       </c>
@@ -1552,7 +1561,7 @@
         <v>68139</v>
       </c>
     </row>
-    <row r="20" spans="2:26" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:26">
       <c r="B20" t="s">
         <v>12</v>
       </c>
@@ -1629,7 +1638,7 @@
         <v>1019</v>
       </c>
     </row>
-    <row r="21" spans="2:26" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:26">
       <c r="B21" t="s">
         <v>13</v>
       </c>
@@ -1706,7 +1715,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="22" spans="2:26" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:26">
       <c r="B22" t="s">
         <v>14</v>
       </c>
@@ -1783,7 +1792,7 @@
         <v>653</v>
       </c>
     </row>
-    <row r="23" spans="2:26" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:26">
       <c r="B23" t="s">
         <v>15</v>
       </c>
@@ -1860,7 +1869,7 @@
         <v>937</v>
       </c>
     </row>
-    <row r="24" spans="2:26" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:26">
       <c r="B24" t="s">
         <v>16</v>
       </c>
@@ -1937,7 +1946,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="25" spans="2:26" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:26">
       <c r="B25" t="s">
         <v>17</v>
       </c>
@@ -2014,7 +2023,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="26" spans="2:26" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:26">
       <c r="B26" t="s">
         <v>18</v>
       </c>
@@ -2091,7 +2100,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="27" spans="2:26" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:26">
       <c r="B27" t="s">
         <v>19</v>
       </c>
@@ -2168,7 +2177,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="28" spans="2:26" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:26">
       <c r="B28" t="s">
         <v>20</v>
       </c>
@@ -2245,7 +2254,7 @@
         <v>787</v>
       </c>
     </row>
-    <row r="29" spans="2:26" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:26">
       <c r="B29" t="s">
         <v>21</v>
       </c>
@@ -2322,7 +2331,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="30" spans="2:26" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:26">
       <c r="B30" t="s">
         <v>22</v>
       </c>
@@ -2399,7 +2408,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="31" spans="2:26" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:26">
       <c r="B31" t="s">
         <v>23</v>
       </c>
@@ -2476,7 +2485,7 @@
         <v>655</v>
       </c>
     </row>
-    <row r="32" spans="2:26" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:26">
       <c r="B32" t="s">
         <v>24</v>
       </c>
@@ -2553,7 +2562,7 @@
         <v>561</v>
       </c>
     </row>
-    <row r="33" spans="2:26" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:26">
       <c r="B33" t="s">
         <v>25</v>
       </c>
@@ -2630,7 +2639,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="34" spans="2:26" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:26">
       <c r="B34" t="s">
         <v>26</v>
       </c>
@@ -2707,7 +2716,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="2:26" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:26">
       <c r="B35" t="s">
         <v>27</v>
       </c>
@@ -2784,7 +2793,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="36" spans="2:26" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:26">
       <c r="B36" t="s">
         <v>28</v>
       </c>
@@ -2861,7 +2870,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="37" spans="2:26" x14ac:dyDescent="0.2">
+    <row r="37" spans="2:26">
       <c r="B37" t="s">
         <v>29</v>
       </c>
@@ -2938,7 +2947,7 @@
         <v>1268</v>
       </c>
     </row>
-    <row r="38" spans="2:26" x14ac:dyDescent="0.2">
+    <row r="38" spans="2:26">
       <c r="B38" t="s">
         <v>30</v>
       </c>
@@ -3015,93 +3024,99 @@
         <v>579</v>
       </c>
     </row>
-    <row r="39" spans="2:26" x14ac:dyDescent="0.2">
+    <row r="39" spans="2:26">
+      <c r="C39">
+        <v>0</v>
+      </c>
+      <c r="D39">
+        <v>0</v>
+      </c>
       <c r="E39">
-        <f>SUM(E8:E38)</f>
+        <f t="shared" ref="E39:Z39" si="0">SUM(E8:E38)</f>
         <v>408</v>
       </c>
       <c r="F39">
-        <f>SUM(F8:F38)</f>
+        <f t="shared" si="0"/>
         <v>34519</v>
       </c>
       <c r="G39">
-        <f>SUM(G8:G38)</f>
+        <f t="shared" si="0"/>
         <v>66434</v>
       </c>
       <c r="H39">
-        <f>SUM(H8:H38)</f>
+        <f t="shared" si="0"/>
         <v>76288</v>
       </c>
       <c r="I39">
-        <f>SUM(I8:I38)</f>
+        <f t="shared" si="0"/>
         <v>80699</v>
       </c>
       <c r="J39">
-        <f>SUM(J8:J38)</f>
+        <f t="shared" si="0"/>
         <v>80844</v>
       </c>
       <c r="K39">
-        <f>SUM(K8:K38)</f>
+        <f t="shared" si="0"/>
         <v>81053</v>
       </c>
       <c r="L39">
-        <f>SUM(L8:L38)</f>
+        <f t="shared" si="0"/>
         <v>81805</v>
       </c>
       <c r="M39">
-        <f>SUM(M8:M38)</f>
+        <f t="shared" si="0"/>
         <v>82295</v>
       </c>
       <c r="N39">
-        <f>SUM(N8:N38)</f>
+        <f t="shared" si="0"/>
         <v>82785</v>
       </c>
       <c r="O39">
-        <f>SUM(O8:O38)</f>
+        <f t="shared" si="0"/>
         <v>82873</v>
       </c>
       <c r="P39">
-        <f>SUM(P8:P38)</f>
+        <f t="shared" si="0"/>
         <v>82899</v>
       </c>
       <c r="Q39">
-        <f>SUM(Q8:Q38)</f>
+        <f t="shared" si="0"/>
         <v>82920</v>
       </c>
       <c r="R39">
-        <f>SUM(R8:R38)</f>
+        <f t="shared" si="0"/>
         <v>82938</v>
       </c>
       <c r="S39">
-        <f>SUM(S8:S38)</f>
+        <f t="shared" si="0"/>
         <v>82938</v>
       </c>
       <c r="T39">
-        <f>SUM(T8:T38)</f>
+        <f t="shared" si="0"/>
         <v>82942</v>
       </c>
       <c r="U39">
-        <f>SUM(U8:U38)</f>
+        <f t="shared" si="0"/>
         <v>82943</v>
       </c>
       <c r="V39">
-        <f>SUM(V8:V38)</f>
+        <f t="shared" si="0"/>
         <v>82943</v>
       </c>
       <c r="W39">
-        <f>SUM(W8:W38)</f>
+        <f t="shared" si="0"/>
         <v>82943</v>
       </c>
       <c r="X39">
-        <f>SUM(X8:X38)</f>
+        <f t="shared" si="0"/>
         <v>82946</v>
       </c>
       <c r="Y39">
-        <f>SUM(Y8:Y38)</f>
+        <f t="shared" si="0"/>
         <v>82947</v>
       </c>
       <c r="Z39">
-        <f>SUM(Z8:Z38)</f>
+        <f t="shared" si="0"/>
         <v>82947</v>
       </c>
     </row>

</xml_diff>